<commit_message>
Auto convert from Jina to YML
</commit_message>
<xml_diff>
--- a/Data/Asplund_2008.xlsx
+++ b/Data/Asplund_2008.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="92">
   <si>
     <t>Z</t>
   </si>
@@ -308,7 +308,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="0.0000000000E+00"/>
+    <numFmt numFmtId="164" formatCode="0.0000000000E+00"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -344,7 +344,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2327,10 +2327,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D287"/>
+  <dimension ref="A1:D288"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2361,24 +2361,24 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>1.4307999611E-5</v>
+        <v>0.71538567254999996</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
       <c r="D3" s="2">
-        <v>4.4869800150000003E-5</v>
+        <v>1.4307999611E-5</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2389,24 +2389,24 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2">
-        <v>0.27025513110999999</v>
+        <v>4.4869800150000003E-5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2">
-        <v>6.4407632918000004E-10</v>
+        <v>0.27025513110999999</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2417,38 +2417,38 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" s="2">
-        <v>9.1487407785000008E-9</v>
+        <v>6.4407632918000004E-10</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2">
-        <v>1.6779801602000001E-10</v>
+        <v>9.1487407785000008E-9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" s="2">
-        <v>7.7517077092000004E-10</v>
+        <v>1.6779801602000001E-10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2459,24 +2459,24 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2">
-        <v>3.4321757097999999E-9</v>
+        <v>7.7517077092000004E-10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C10">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2">
-        <v>2.4825306734E-3</v>
+        <v>3.4321757097999999E-9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2487,24 +2487,24 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2">
-        <v>3.0083012114999999E-5</v>
+        <v>2.4825306734E-3</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2">
-        <v>7.3396723494000005E-4</v>
+        <v>3.0083012114999999E-5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2515,24 +2515,24 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="2">
-        <v>1.8049744286000001E-6</v>
+        <v>7.3396723494000005E-4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C14">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D14" s="2">
-        <v>6.0761694571000004E-3</v>
+        <v>1.8049744286000001E-6</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -2543,10 +2543,10 @@
         <v>18</v>
       </c>
       <c r="C15">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2">
-        <v>2.4526323005E-6</v>
+        <v>6.0761694571000004E-3</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -2557,38 +2557,38 @@
         <v>18</v>
       </c>
       <c r="C16">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D16" s="2">
-        <v>1.3703983054E-5</v>
+        <v>2.4526323005E-6</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="2">
-        <v>5.3616432418999999E-7</v>
+        <v>1.3703983054E-5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C18">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="2">
-        <v>1.2296781652000001E-3</v>
+        <v>5.3616432418999999E-7</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -2599,10 +2599,10 @@
         <v>22</v>
       </c>
       <c r="C19">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D19" s="2">
-        <v>3.0951292776999999E-6</v>
+        <v>1.2296781652000001E-3</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -2613,38 +2613,38 @@
         <v>22</v>
       </c>
       <c r="C20">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D20" s="2">
-        <v>9.9459969635000002E-5</v>
+        <v>3.0951292776999999E-6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C21">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D21" s="2">
-        <v>3.1065056525000001E-5</v>
+        <v>9.9459969635000002E-5</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C22">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="2">
-        <v>5.8658056252000005E-4</v>
+        <v>3.1065056525000001E-5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2655,10 +2655,10 @@
         <v>26</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="2">
-        <v>7.7354275135000007E-5</v>
+        <v>5.8658056252000005E-4</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2669,38 +2669,38 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" s="2">
-        <v>8.8573739201000006E-5</v>
+        <v>7.7354275135000007E-5</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C25">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="2">
-        <v>5.9143643625000003E-5</v>
+        <v>8.8573739201000006E-5</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C26">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2">
-        <v>6.4949100307999999E-4</v>
+        <v>5.9143643625000003E-5</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -2711,10 +2711,10 @@
         <v>30</v>
       </c>
       <c r="C27">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D27" s="2">
-        <v>3.4157416484000003E-5</v>
+        <v>6.4949100307999999E-4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -2725,38 +2725,38 @@
         <v>30</v>
       </c>
       <c r="C28">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="2">
-        <v>2.3293263116999998E-5</v>
+        <v>3.4157416484000003E-5</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C29">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="2">
-        <v>6.1930702445000003E-6</v>
+        <v>2.3293263116999998E-5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C30">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D30" s="2">
-        <v>3.1124169468999999E-4</v>
+        <v>6.1930702445000003E-6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2767,10 +2767,10 @@
         <v>34</v>
       </c>
       <c r="C31">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="2">
-        <v>2.5696373982E-6</v>
+        <v>3.1124169468999999E-4</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -2781,10 +2781,10 @@
         <v>34</v>
       </c>
       <c r="C32">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="2">
-        <v>1.4944470132E-5</v>
+        <v>2.5696373982E-6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2795,24 +2795,24 @@
         <v>34</v>
       </c>
       <c r="C33">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D33" s="2">
-        <v>7.3769494686000002E-8</v>
+        <v>1.4944470132E-5</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34">
         <v>36</v>
       </c>
-      <c r="C34">
-        <v>35</v>
-      </c>
       <c r="D34" s="2">
-        <v>6.5187895016000001E-6</v>
+        <v>7.3769494686000002E-8</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2823,24 +2823,24 @@
         <v>36</v>
       </c>
       <c r="C35">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D35" s="2">
-        <v>2.2025215941000001E-6</v>
+        <v>6.5187895016000001E-6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C36">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D36" s="2">
-        <v>5.9455146581000002E-5</v>
+        <v>2.2025215941000001E-6</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2851,10 +2851,10 @@
         <v>38</v>
       </c>
       <c r="C37">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D37" s="2">
-        <v>1.141055671E-5</v>
+        <v>5.9455146581000002E-5</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2865,24 +2865,24 @@
         <v>38</v>
       </c>
       <c r="C38">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D38" s="2">
-        <v>1.9210532821999999E-8</v>
+        <v>1.141055671E-5</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39">
         <v>40</v>
       </c>
-      <c r="C39">
-        <v>39</v>
-      </c>
       <c r="D39" s="2">
-        <v>3.0248778981999998E-6</v>
+        <v>1.9210532821999999E-8</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -2893,10 +2893,10 @@
         <v>40</v>
       </c>
       <c r="C40">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D40" s="2">
-        <v>4.8969045428E-9</v>
+        <v>3.0248778981999998E-6</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -2907,24 +2907,24 @@
         <v>40</v>
       </c>
       <c r="C41">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D41" s="2">
-        <v>2.294891008E-7</v>
+        <v>4.8969045428E-9</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C42">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D42" s="2">
-        <v>6.5934360588000007E-5</v>
+        <v>2.294891008E-7</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2935,10 +2935,10 @@
         <v>42</v>
       </c>
       <c r="C43">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D43" s="2">
-        <v>4.6205947809000001E-7</v>
+        <v>6.5934360588000007E-5</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -2949,10 +2949,10 @@
         <v>42</v>
       </c>
       <c r="C44">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D44" s="2">
-        <v>9.8706678086000005E-8</v>
+        <v>4.6205947809000001E-7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -2963,10 +2963,10 @@
         <v>42</v>
       </c>
       <c r="C45">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D45" s="2">
-        <v>1.5606707564999999E-6</v>
+        <v>9.8706678086000005E-8</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -2977,10 +2977,10 @@
         <v>42</v>
       </c>
       <c r="C46">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D46" s="2">
-        <v>3.1286871261999998E-9</v>
+        <v>1.5606707564999999E-6</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -2991,38 +2991,38 @@
         <v>42</v>
       </c>
       <c r="C47">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D47" s="2">
-        <v>1.5262551980999999E-7</v>
+        <v>3.1286871261999998E-9</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C48">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D48" s="2">
-        <v>4.9403398557999997E-8</v>
+        <v>1.5262551980999999E-7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C49">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D49" s="2">
-        <v>2.6287912006999999E-7</v>
+        <v>4.9403398557999997E-8</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -3033,10 +3033,10 @@
         <v>46</v>
       </c>
       <c r="C50">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D50" s="2">
-        <v>2.4222284771000002E-7</v>
+        <v>2.6287912006999999E-7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -3047,10 +3047,10 @@
         <v>46</v>
       </c>
       <c r="C51">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D51" s="2">
-        <v>2.4511555708000001E-6</v>
+        <v>2.4222284771000002E-7</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -3061,10 +3061,10 @@
         <v>46</v>
       </c>
       <c r="C52">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D52" s="2">
-        <v>1.8362747282999999E-7</v>
+        <v>2.4511555708000001E-6</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -3075,24 +3075,24 @@
         <v>46</v>
       </c>
       <c r="C53">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D53" s="2">
-        <v>1.7940893834000001E-7</v>
+        <v>1.8362747282999999E-7</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C54">
         <v>50</v>
       </c>
       <c r="D54" s="2">
-        <v>8.2690253850000004E-10</v>
+        <v>1.7940893834000001E-7</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3103,24 +3103,24 @@
         <v>48</v>
       </c>
       <c r="C55">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D55" s="2">
-        <v>3.3653279511999999E-7</v>
+        <v>8.2690253850000004E-10</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C56">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D56" s="2">
-        <v>7.3706212899999995E-7</v>
+        <v>3.3653279511999999E-7</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -3131,10 +3131,10 @@
         <v>50</v>
       </c>
       <c r="C57">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D57" s="2">
-        <v>1.4782049868E-5</v>
+        <v>7.3706212899999995E-7</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -3145,10 +3145,10 @@
         <v>50</v>
       </c>
       <c r="C58">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D58" s="2">
-        <v>1.7083997526E-6</v>
+        <v>1.4782049868E-5</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -3159,38 +3159,38 @@
         <v>50</v>
       </c>
       <c r="C59">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D59" s="2">
-        <v>4.3328057305000002E-7</v>
+        <v>1.7083997526E-6</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C60">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D60" s="2">
-        <v>1.1505539868E-5</v>
+        <v>4.3328057305000002E-7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C61">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D61" s="2">
-        <v>7.7575143475000003E-5</v>
+        <v>1.1505539868E-5</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -3201,10 +3201,10 @@
         <v>54</v>
       </c>
       <c r="C62">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D62" s="2">
-        <v>1.2628662167999999E-3</v>
+        <v>7.7575143475000003E-5</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3215,10 +3215,10 @@
         <v>54</v>
       </c>
       <c r="C63">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D63" s="2">
-        <v>2.9685893465000001E-5</v>
+        <v>1.2628662167999999E-3</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -3229,38 +3229,38 @@
         <v>54</v>
       </c>
       <c r="C64">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D64" s="2">
-        <v>4.0199570594000001E-6</v>
+        <v>2.9685893465000001E-5</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C65">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D65" s="2">
-        <v>4.4812206005999998E-6</v>
+        <v>4.0199570594000001E-6</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C66">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D66" s="2">
-        <v>5.0929812451999997E-5</v>
+        <v>4.4812206005999998E-6</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -3271,10 +3271,10 @@
         <v>58</v>
       </c>
       <c r="C67">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D67" s="2">
-        <v>2.0294557837000001E-5</v>
+        <v>5.0929812451999997E-5</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -3285,10 +3285,10 @@
         <v>58</v>
       </c>
       <c r="C68">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D68" s="2">
-        <v>8.9689355006000005E-7</v>
+        <v>2.0294557837000001E-5</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -3299,10 +3299,10 @@
         <v>58</v>
       </c>
       <c r="C69">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D69" s="2">
-        <v>2.9065692514999999E-6</v>
+        <v>8.9689355006000005E-7</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -3313,24 +3313,24 @@
         <v>58</v>
       </c>
       <c r="C70">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D70" s="2">
-        <v>7.6409548256999996E-7</v>
+        <v>2.9065692514999999E-6</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C71">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D71" s="2">
-        <v>5.2456901860999996E-7</v>
+        <v>7.6409548256999996E-7</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -3341,24 +3341,24 @@
         <v>60</v>
       </c>
       <c r="C72">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D72" s="2">
-        <v>2.4122993150999998E-7</v>
+        <v>5.2456901860999996E-7</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C73">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D73" s="2">
-        <v>8.7827102604000002E-7</v>
+        <v>2.4122993150999998E-7</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -3369,10 +3369,10 @@
         <v>62</v>
       </c>
       <c r="C74">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D74" s="2">
-        <v>5.1962788767E-7</v>
+        <v>8.7827102604000002E-7</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -3383,10 +3383,10 @@
         <v>62</v>
       </c>
       <c r="C75">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D75" s="2">
-        <v>7.7518073608000005E-8</v>
+        <v>5.1962788767E-7</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3397,10 +3397,10 @@
         <v>62</v>
       </c>
       <c r="C76">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D76" s="2">
-        <v>3.5979448070999998E-7</v>
+        <v>7.7518073608000005E-8</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -3411,24 +3411,24 @@
         <v>62</v>
       </c>
       <c r="C77">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D77" s="2">
-        <v>1.2247121931999999E-8</v>
+        <v>3.5979448070999998E-7</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C78">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D78" s="2">
-        <v>3.5344812378999998E-8</v>
+        <v>1.2247121931999999E-8</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -3439,24 +3439,24 @@
         <v>64</v>
       </c>
       <c r="C79">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D79" s="2">
-        <v>2.4137287938E-8</v>
+        <v>3.5344812378999998E-8</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C80">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D80" s="2">
-        <v>5.0645407140999998E-8</v>
+        <v>2.4137287938E-8</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -3467,10 +3467,10 @@
         <v>66</v>
       </c>
       <c r="C81">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D81" s="2">
-        <v>6.8839981431999995E-8</v>
+        <v>5.0645407140999998E-8</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -3481,10 +3481,10 @@
         <v>66</v>
       </c>
       <c r="C82">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D82" s="2">
-        <v>1.9590551683E-8</v>
+        <v>6.8839981431999995E-8</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -3495,10 +3495,10 @@
         <v>66</v>
       </c>
       <c r="C83">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D83" s="2">
-        <v>9.3205879806000003E-8</v>
+        <v>1.9590551683E-8</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -3509,38 +3509,38 @@
         <v>66</v>
       </c>
       <c r="C84">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D84" s="2">
-        <v>2.0079022260999999E-8</v>
+        <v>9.3205879806000003E-8</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C85">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D85" s="2">
-        <v>1.1630692549E-8</v>
+        <v>2.0079022260999999E-8</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C86">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D86" s="2">
-        <v>1.1198659464000001E-9</v>
+        <v>1.1630692549E-8</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3551,10 +3551,10 @@
         <v>70</v>
       </c>
       <c r="C87">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D87" s="2">
-        <v>1.2108699328E-8</v>
+        <v>1.1198659464000001E-9</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -3565,10 +3565,10 @@
         <v>70</v>
       </c>
       <c r="C88">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D88" s="2">
-        <v>9.9898639866000001E-9</v>
+        <v>1.2108699328E-8</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -3579,10 +3579,10 @@
         <v>70</v>
       </c>
       <c r="C89">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D89" s="2">
-        <v>3.1525943768000001E-8</v>
+        <v>9.9898639866000001E-9</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -3593,10 +3593,10 @@
         <v>70</v>
       </c>
       <c r="C90">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D90" s="2">
-        <v>6.7484421014000001E-8</v>
+        <v>3.1525943768000001E-8</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -3607,24 +3607,24 @@
         <v>70</v>
       </c>
       <c r="C91">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D91" s="2">
-        <v>1.2172293295E-8</v>
+        <v>6.7484421014000001E-8</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C92">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D92" s="2">
-        <v>1.0791795193E-8</v>
+        <v>1.2172293295E-8</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -3635,24 +3635,24 @@
         <v>72</v>
       </c>
       <c r="C93">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D93" s="2">
-        <v>1.0763768126000001E-8</v>
+        <v>1.0791795193E-8</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C94">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D94" s="2">
-        <v>3.9025410982999999E-10</v>
+        <v>1.0763768126000001E-8</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -3663,10 +3663,10 @@
         <v>74</v>
       </c>
       <c r="C95">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D95" s="2">
-        <v>2.5718403724999998E-9</v>
+        <v>3.9025410982999999E-10</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3677,10 +3677,10 @@
         <v>74</v>
       </c>
       <c r="C96">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D96" s="2">
-        <v>1.3209015275000001E-8</v>
+        <v>2.5718403724999998E-9</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3691,10 +3691,10 @@
         <v>74</v>
       </c>
       <c r="C97">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D97" s="2">
-        <v>1.3245060845E-8</v>
+        <v>1.3209015275000001E-8</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -3705,10 +3705,10 @@
         <v>74</v>
       </c>
       <c r="C98">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D98" s="2">
-        <v>6.6063071518000001E-8</v>
+        <v>1.3245060845E-8</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -3719,24 +3719,24 @@
         <v>74</v>
       </c>
       <c r="C99">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D99" s="2">
-        <v>2.0453760238000001E-8</v>
+        <v>6.6063071518000001E-8</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C100">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D100" s="2">
-        <v>1.5497666547999999E-8</v>
+        <v>2.0453760238000001E-8</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -3747,24 +3747,24 @@
         <v>76</v>
       </c>
       <c r="C101">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D101" s="2">
-        <v>6.5281707664000001E-9</v>
+        <v>1.5497666547999999E-8</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C102">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="D102" s="2">
-        <v>2.7005846645999997E-10</v>
+        <v>6.5281707664000001E-9</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3775,10 +3775,10 @@
         <v>78</v>
       </c>
       <c r="C103">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D103" s="2">
-        <v>4.8894848190000002E-9</v>
+        <v>2.7005846645999997E-10</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -3789,10 +3789,10 @@
         <v>78</v>
       </c>
       <c r="C104">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D104" s="2">
-        <v>3.4567431852000001E-9</v>
+        <v>4.8894848190000002E-9</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -3803,38 +3803,38 @@
         <v>78</v>
       </c>
       <c r="C105">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D105" s="2">
-        <v>4.1919633017999999E-8</v>
+        <v>3.4567431852000001E-9</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C106">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D106" s="2">
-        <v>1.1218487769E-8</v>
+        <v>4.1919633017999999E-8</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C107">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D107" s="2">
-        <v>1.3682712469000001E-8</v>
+        <v>1.1218487769E-8</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -3845,10 +3845,10 @@
         <v>82</v>
       </c>
       <c r="C108">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D108" s="2">
-        <v>3.017022586E-9</v>
+        <v>1.3682712469000001E-8</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -3859,10 +3859,10 @@
         <v>82</v>
       </c>
       <c r="C109">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D109" s="2">
-        <v>4.6622575819000003E-9</v>
+        <v>3.017022586E-9</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3873,10 +3873,10 @@
         <v>82</v>
       </c>
       <c r="C110">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D110" s="2">
-        <v>4.8274961698E-9</v>
+        <v>4.6622575819000003E-9</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3887,38 +3887,38 @@
         <v>82</v>
       </c>
       <c r="C111">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D111" s="2">
-        <v>7.9427990747000004E-10</v>
+        <v>4.8274961698E-9</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C112">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D112" s="2">
-        <v>2.0846217309E-9</v>
+        <v>7.9427990747000004E-10</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C113">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D113" s="2">
-        <v>7.8785860104999999E-10</v>
+        <v>2.0846217309E-9</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -3929,10 +3929,10 @@
         <v>86</v>
       </c>
       <c r="C114">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D114" s="2">
-        <v>5.0715501120000005E-10</v>
+        <v>7.8785860104999999E-10</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -3943,10 +3943,10 @@
         <v>86</v>
       </c>
       <c r="C115">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D115" s="2">
-        <v>8.8709116943999999E-10</v>
+        <v>5.0715501120000005E-10</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -3957,10 +3957,10 @@
         <v>86</v>
       </c>
       <c r="C116">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D116" s="2">
-        <v>9.4363327493000003E-10</v>
+        <v>8.8709116943999999E-10</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -3971,10 +3971,10 @@
         <v>86</v>
       </c>
       <c r="C117">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D117" s="2">
-        <v>5.4896169049999999E-10</v>
+        <v>9.4363327493000003E-10</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -3985,10 +3985,10 @@
         <v>86</v>
       </c>
       <c r="C118">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D118" s="2">
-        <v>1.4092887790999999E-9</v>
+        <v>5.4896169049999999E-10</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -3999,24 +3999,24 @@
         <v>86</v>
       </c>
       <c r="C119">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D119" s="2">
-        <v>5.7920548505000002E-10</v>
+        <v>1.4092887790999999E-9</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>5</v>
+        <v>86</v>
       </c>
       <c r="C120">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D120" s="2">
-        <v>2.3244773028999999E-10</v>
+        <v>5.7920548505000002E-10</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -4027,10 +4027,10 @@
         <v>5</v>
       </c>
       <c r="C121">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D121" s="2">
-        <v>8.0096215128000002E-11</v>
+        <v>2.3244773028999999E-10</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -4041,10 +4041,10 @@
         <v>5</v>
       </c>
       <c r="C122">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D122" s="2">
-        <v>5.5211580704000004E-10</v>
+        <v>8.0096215128000002E-11</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -4055,10 +4055,10 @@
         <v>5</v>
       </c>
       <c r="C123">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D123" s="2">
-        <v>5.5069972204000003E-10</v>
+        <v>5.5211580704000004E-10</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -4069,10 +4069,10 @@
         <v>5</v>
       </c>
       <c r="C124">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D124" s="2">
-        <v>7.5308624052999998E-10</v>
+        <v>5.5069972204000003E-10</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -4083,10 +4083,10 @@
         <v>5</v>
       </c>
       <c r="C125">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D125" s="2">
-        <v>1.4065133139E-9</v>
+        <v>7.5308624052999998E-10</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -4097,38 +4097,38 @@
         <v>5</v>
       </c>
       <c r="C126">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D126" s="2">
-        <v>8.4636428392000003E-10</v>
+        <v>1.4065133139E-9</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C127">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D127" s="2">
-        <v>6.5070109395000004E-10</v>
+        <v>8.4636428392000003E-10</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C128">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D128" s="2">
-        <v>3.0043093935000002E-11</v>
+        <v>6.5070109395000004E-10</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -4139,10 +4139,10 @@
         <v>9</v>
       </c>
       <c r="C129">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D129" s="2">
-        <v>3.3455139281999999E-10</v>
+        <v>3.0043093935000002E-11</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -4153,10 +4153,10 @@
         <v>9</v>
       </c>
       <c r="C130">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D130" s="2">
-        <v>6.7705248168000004E-10</v>
+        <v>3.3455139281999999E-10</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -4167,10 +4167,10 @@
         <v>9</v>
       </c>
       <c r="C131">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D131" s="2">
-        <v>8.3654596565999995E-10</v>
+        <v>6.7705248168000004E-10</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -4181,10 +4181,10 @@
         <v>9</v>
       </c>
       <c r="C132">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D132" s="2">
-        <v>8.2519750746000004E-10</v>
+        <v>8.3654596565999995E-10</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -4195,24 +4195,24 @@
         <v>9</v>
       </c>
       <c r="C133">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D133" s="2">
-        <v>3.7227563150000002E-10</v>
+        <v>8.2519750746000004E-10</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C134">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D134" s="2">
-        <v>3.7547818080000001E-10</v>
+        <v>3.7227563150000002E-10</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -4223,24 +4223,24 @@
         <v>11</v>
       </c>
       <c r="C135">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D135" s="2">
-        <v>3.5535817106000002E-10</v>
+        <v>3.7547818080000001E-10</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C136">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D136" s="2">
-        <v>5.2815353440000003E-11</v>
+        <v>3.5535817106000002E-10</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -4251,10 +4251,10 @@
         <v>13</v>
       </c>
       <c r="C137">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D137" s="2">
-        <v>3.8314051115E-11</v>
+        <v>5.2815353440000003E-11</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -4265,10 +4265,10 @@
         <v>13</v>
       </c>
       <c r="C138">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D138" s="2">
-        <v>5.4764538937000002E-10</v>
+        <v>3.8314051115E-11</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -4279,10 +4279,10 @@
         <v>13</v>
       </c>
       <c r="C139">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D139" s="2">
-        <v>5.6634003146E-10</v>
+        <v>5.4764538937000002E-10</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -4293,10 +4293,10 @@
         <v>13</v>
       </c>
       <c r="C140">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D140" s="2">
-        <v>1.0772578232999999E-9</v>
+        <v>5.6634003146E-10</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -4307,10 +4307,10 @@
         <v>13</v>
       </c>
       <c r="C141">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D141" s="2">
-        <v>5.5041969019999998E-10</v>
+        <v>1.0772578232999999E-9</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -4321,10 +4321,10 @@
         <v>13</v>
       </c>
       <c r="C142">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D142" s="2">
-        <v>1.3055237879E-9</v>
+        <v>5.5041969019999998E-10</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -4335,24 +4335,24 @@
         <v>13</v>
       </c>
       <c r="C143">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D143" s="2">
-        <v>3.4632522025000003E-10</v>
+        <v>1.3055237879E-9</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C144">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D144" s="2">
-        <v>2.3772784189000001E-11</v>
+        <v>3.4632522025000003E-10</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -4363,24 +4363,24 @@
         <v>15</v>
       </c>
       <c r="C145">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D145" s="2">
-        <v>5.3975847328999995E-10</v>
+        <v>2.3772784189000001E-11</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C146">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D146" s="2">
-        <v>9.2583601132000005E-11</v>
+        <v>5.3975847328999995E-10</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -4391,10 +4391,10 @@
         <v>17</v>
       </c>
       <c r="C147">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D147" s="2">
-        <v>6.4119938780999995E-11</v>
+        <v>9.2583601132000005E-11</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -4405,10 +4405,10 @@
         <v>17</v>
       </c>
       <c r="C148">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D148" s="2">
-        <v>3.3321233471000003E-11</v>
+        <v>6.4119938780999995E-11</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -4419,10 +4419,10 @@
         <v>17</v>
       </c>
       <c r="C149">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D149" s="2">
-        <v>1.4373638163999999E-9</v>
+        <v>3.3321233471000003E-11</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -4433,10 +4433,10 @@
         <v>17</v>
       </c>
       <c r="C150">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D150" s="2">
-        <v>7.6575773778999996E-10</v>
+        <v>1.4373638163999999E-9</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -4447,10 +4447,10 @@
         <v>17</v>
       </c>
       <c r="C151">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D151" s="2">
-        <v>2.4355691154000001E-9</v>
+        <v>7.6575773778999996E-10</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -4461,10 +4461,10 @@
         <v>17</v>
       </c>
       <c r="C152">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D152" s="2">
-        <v>8.7113294286999995E-10</v>
+        <v>2.4355691154000001E-9</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
@@ -4475,10 +4475,10 @@
         <v>17</v>
       </c>
       <c r="C153">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D153" s="2">
-        <v>3.3317824649E-9</v>
+        <v>8.7113294286999995E-10</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -4489,10 +4489,10 @@
         <v>17</v>
       </c>
       <c r="C154">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D154" s="2">
-        <v>4.8137677592000005E-10</v>
+        <v>3.3317824649E-9</v>
       </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
@@ -4503,24 +4503,24 @@
         <v>17</v>
       </c>
       <c r="C155">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D155" s="2">
-        <v>6.1184943177999999E-10</v>
+        <v>4.8137677592000005E-10</v>
       </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C156">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D156" s="2">
-        <v>5.5055616513999999E-10</v>
+        <v>6.1184943177999999E-10</v>
       </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
@@ -4531,24 +4531,24 @@
         <v>19</v>
       </c>
       <c r="C157">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D157" s="2">
-        <v>4.1859275768000001E-10</v>
+        <v>5.5055616513999999E-10</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C158">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="D158" s="2">
-        <v>1.2704806872000001E-11</v>
+        <v>4.1859275768000001E-10</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -4559,10 +4559,10 @@
         <v>21</v>
       </c>
       <c r="C159">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D159" s="2">
-        <v>3.6596902016999999E-10</v>
+        <v>1.2704806872000001E-11</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -4573,10 +4573,10 @@
         <v>21</v>
       </c>
       <c r="C160">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D160" s="2">
-        <v>1.287773341E-10</v>
+        <v>3.6596902016999999E-10</v>
       </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
@@ -4587,10 +4587,10 @@
         <v>21</v>
       </c>
       <c r="C161">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D161" s="2">
-        <v>6.9142382286999995E-10</v>
+        <v>1.287773341E-10</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
@@ -4601,10 +4601,10 @@
         <v>21</v>
       </c>
       <c r="C162">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D162" s="2">
-        <v>1.0396178770999999E-9</v>
+        <v>6.9142382286999995E-10</v>
       </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
@@ -4615,10 +4615,10 @@
         <v>21</v>
       </c>
       <c r="C163">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D163" s="2">
-        <v>2.7925165504000001E-9</v>
+        <v>1.0396178770999999E-9</v>
       </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
@@ -4629,10 +4629,10 @@
         <v>21</v>
       </c>
       <c r="C164">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D164" s="2">
-        <v>4.7792660162000003E-9</v>
+        <v>2.7925165504000001E-9</v>
       </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
@@ -4643,38 +4643,38 @@
         <v>21</v>
       </c>
       <c r="C165">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D165" s="2">
-        <v>5.2117941079000003E-9</v>
+        <v>4.7792660162000003E-9</v>
       </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C166">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D166" s="2">
-        <v>3.5022571704E-9</v>
+        <v>5.2117941079000003E-9</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C167">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D167" s="2">
-        <v>2.0432703265999999E-11</v>
+        <v>3.5022571704E-9</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -4685,10 +4685,10 @@
         <v>25</v>
       </c>
       <c r="C168">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D168" s="2">
-        <v>1.8379708226000001E-11</v>
+        <v>2.0432703265999999E-11</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -4699,10 +4699,10 @@
         <v>25</v>
       </c>
       <c r="C169">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D169" s="2">
-        <v>3.7826973872E-10</v>
+        <v>1.8379708226000001E-11</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -4713,10 +4713,10 @@
         <v>25</v>
       </c>
       <c r="C170">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D170" s="2">
-        <v>4.7487598657000001E-9</v>
+        <v>3.7826973872E-10</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,10 +4727,10 @@
         <v>25</v>
       </c>
       <c r="C171">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D171" s="2">
-        <v>7.6836040678E-10</v>
+        <v>4.7487598657000001E-9</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -4741,10 +4741,10 @@
         <v>25</v>
       </c>
       <c r="C172">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D172" s="2">
-        <v>3.8382673706999998E-9</v>
+        <v>7.6836040678E-10</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -4755,10 +4755,10 @@
         <v>25</v>
       </c>
       <c r="C173">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D173" s="2">
-        <v>4.7270859108000001E-9</v>
+        <v>3.8382673706999998E-9</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -4769,10 +4769,10 @@
         <v>25</v>
       </c>
       <c r="C174">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D174" s="2">
-        <v>1.7718697849E-9</v>
+        <v>4.7270859108000001E-9</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -4783,38 +4783,38 @@
         <v>25</v>
       </c>
       <c r="C175">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D175" s="2">
-        <v>1.4610625437E-9</v>
+        <v>1.7718697849E-9</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C176">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D176" s="2">
-        <v>1.2427848577999999E-9</v>
+        <v>1.4610625437E-9</v>
       </c>
     </row>
     <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B177" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C177">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="D177" s="2">
-        <v>1.6210392471999999E-11</v>
+        <v>1.2427848577999999E-9</v>
       </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
@@ -4825,10 +4825,10 @@
         <v>29</v>
       </c>
       <c r="C178">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D178" s="2">
-        <v>1.5683378261000001E-11</v>
+        <v>1.6210392471999999E-11</v>
       </c>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
@@ -4839,10 +4839,10 @@
         <v>29</v>
       </c>
       <c r="C179">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D179" s="2">
-        <v>3.8100068888999998E-10</v>
+        <v>1.5683378261000001E-11</v>
       </c>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
@@ -4853,10 +4853,10 @@
         <v>29</v>
       </c>
       <c r="C180">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D180" s="2">
-        <v>1.0468760862000001E-9</v>
+        <v>3.8100068888999998E-10</v>
       </c>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
@@ -4867,10 +4867,10 @@
         <v>29</v>
       </c>
       <c r="C181">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D181" s="2">
-        <v>1.2565336325E-9</v>
+        <v>1.0468760862000001E-9</v>
       </c>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
@@ -4881,10 +4881,10 @@
         <v>29</v>
       </c>
       <c r="C182">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D182" s="2">
-        <v>1.8101808831E-9</v>
+        <v>1.2565336325E-9</v>
       </c>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
@@ -4895,24 +4895,24 @@
         <v>29</v>
       </c>
       <c r="C183">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D183" s="2">
-        <v>1.1639395884000001E-8</v>
+        <v>1.8101808831E-9</v>
       </c>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B184" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C184">
         <v>138</v>
       </c>
       <c r="D184" s="2">
-        <v>1.2287535649999999E-12</v>
+        <v>1.1639395884000001E-8</v>
       </c>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
@@ -4923,24 +4923,24 @@
         <v>31</v>
       </c>
       <c r="C185">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D185" s="2">
-        <v>1.3588256131999999E-9</v>
+        <v>1.2287535649999999E-12</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C186">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D186" s="2">
-        <v>7.4345544909999997E-12</v>
+        <v>1.3588256131999999E-9</v>
       </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
@@ -4951,10 +4951,10 @@
         <v>33</v>
       </c>
       <c r="C187">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D187" s="2">
-        <v>1.023521854E-11</v>
+        <v>7.4345544909999997E-12</v>
       </c>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
@@ -4965,10 +4965,10 @@
         <v>33</v>
       </c>
       <c r="C188">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D188" s="2">
-        <v>3.6590655111999999E-9</v>
+        <v>1.023521854E-11</v>
       </c>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
@@ -4979,38 +4979,38 @@
         <v>33</v>
       </c>
       <c r="C189">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D189" s="2">
-        <v>4.6634040870999998E-10</v>
+        <v>3.6590655111999999E-9</v>
       </c>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C190">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D190" s="2">
-        <v>5.7512656071999996E-10</v>
+        <v>4.6634040870999998E-10</v>
       </c>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B191" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C191">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D191" s="2">
-        <v>7.8506132654999997E-10</v>
+        <v>5.7512656071999996E-10</v>
       </c>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
@@ -5021,10 +5021,10 @@
         <v>37</v>
       </c>
       <c r="C192">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D192" s="2">
-        <v>3.5147399415E-10</v>
+        <v>7.8506132654999997E-10</v>
       </c>
     </row>
     <row r="193" spans="1:4" x14ac:dyDescent="0.25">
@@ -5035,10 +5035,10 @@
         <v>37</v>
       </c>
       <c r="C193">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D193" s="2">
-        <v>6.9853189464999996E-10</v>
+        <v>3.5147399415E-10</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -5049,10 +5049,10 @@
         <v>37</v>
       </c>
       <c r="C194">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D194" s="2">
-        <v>2.5975572375999999E-10</v>
+        <v>6.9853189464999996E-10</v>
       </c>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
@@ -5063,10 +5063,10 @@
         <v>37</v>
       </c>
       <c r="C195">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D195" s="2">
-        <v>5.1127496883000001E-10</v>
+        <v>2.5975572375999999E-10</v>
       </c>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
@@ -5077,10 +5077,10 @@
         <v>37</v>
       </c>
       <c r="C196">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D196" s="2">
-        <v>1.7294111222E-10</v>
+        <v>5.1127496883000001E-10</v>
       </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
@@ -5091,24 +5091,24 @@
         <v>37</v>
       </c>
       <c r="C197">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D197" s="2">
-        <v>1.7159841695E-10</v>
+        <v>1.7294111222E-10</v>
       </c>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B198" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C198">
-        <v>144</v>
+        <v>150</v>
       </c>
       <c r="D198" s="2">
-        <v>3.1336116974999997E-11</v>
+        <v>1.7159841695E-10</v>
       </c>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
@@ -5119,10 +5119,10 @@
         <v>39</v>
       </c>
       <c r="C199">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D199" s="2">
-        <v>1.5619361618000001E-10</v>
+        <v>3.1336116974999997E-11</v>
       </c>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
@@ -5133,10 +5133,10 @@
         <v>39</v>
       </c>
       <c r="C200">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D200" s="2">
-        <v>1.1791589149000001E-10</v>
+        <v>1.5619361618000001E-10</v>
       </c>
     </row>
     <row r="201" spans="1:4" x14ac:dyDescent="0.25">
@@ -5147,10 +5147,10 @@
         <v>39</v>
       </c>
       <c r="C201">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D201" s="2">
-        <v>1.4596160277000001E-10</v>
+        <v>1.1791589149000001E-10</v>
       </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
@@ -5161,10 +5161,10 @@
         <v>39</v>
       </c>
       <c r="C202">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D202" s="2">
-        <v>7.8467882490999994E-11</v>
+        <v>1.4596160277000001E-10</v>
       </c>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
@@ -5175,10 +5175,10 @@
         <v>39</v>
       </c>
       <c r="C203">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D203" s="2">
-        <v>2.8821175267000002E-10</v>
+        <v>7.8467882490999994E-11</v>
       </c>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
@@ -5189,24 +5189,24 @@
         <v>39</v>
       </c>
       <c r="C204">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D204" s="2">
-        <v>2.4833986115999998E-10</v>
+        <v>2.8821175267000002E-10</v>
       </c>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C205">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="D205" s="2">
-        <v>1.8579755866000001E-10</v>
+        <v>2.4833986115999998E-10</v>
       </c>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -5217,24 +5217,24 @@
         <v>41</v>
       </c>
       <c r="C206">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D206" s="2">
-        <v>2.0550530614E-10</v>
+        <v>1.8579755866000001E-10</v>
       </c>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C207">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D207" s="2">
-        <v>2.7759899901000001E-12</v>
+        <v>2.0550530614E-10</v>
       </c>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
@@ -5245,10 +5245,10 @@
         <v>43</v>
       </c>
       <c r="C208">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D208" s="2">
-        <v>3.0656426298999999E-11</v>
+        <v>2.7759899901000001E-12</v>
       </c>
     </row>
     <row r="209" spans="1:4" x14ac:dyDescent="0.25">
@@ -5259,10 +5259,10 @@
         <v>43</v>
       </c>
       <c r="C209">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D209" s="2">
-        <v>2.0947766569999999E-10</v>
+        <v>3.0656426298999999E-11</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -5273,10 +5273,10 @@
         <v>43</v>
       </c>
       <c r="C210">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D210" s="2">
-        <v>2.9159948536999999E-10</v>
+        <v>2.0947766569999999E-10</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5287,10 +5287,10 @@
         <v>43</v>
       </c>
       <c r="C211">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D211" s="2">
-        <v>2.2436665149000001E-10</v>
+        <v>2.9159948536999999E-10</v>
       </c>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
@@ -5301,10 +5301,10 @@
         <v>43</v>
       </c>
       <c r="C212">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D212" s="2">
-        <v>3.5838761296E-10</v>
+        <v>2.2436665149000001E-10</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5315,38 +5315,38 @@
         <v>43</v>
       </c>
       <c r="C213">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D213" s="2">
-        <v>3.193849536E-10</v>
+        <v>3.5838761296E-10</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B214" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C214">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D214" s="2">
-        <v>2.4657068204E-10</v>
+        <v>3.193849536E-10</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B215" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C215">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D215" s="2">
-        <v>8.5478508873000003E-13</v>
+        <v>2.4657068204E-10</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5357,10 +5357,10 @@
         <v>47</v>
       </c>
       <c r="C216">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D216" s="2">
-        <v>1.4686726399000001E-12</v>
+        <v>8.5478508873000003E-13</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5371,10 +5371,10 @@
         <v>47</v>
       </c>
       <c r="C217">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D217" s="2">
-        <v>3.6461437209999998E-11</v>
+        <v>1.4686726399000001E-12</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5385,10 +5385,10 @@
         <v>47</v>
       </c>
       <c r="C218">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D218" s="2">
-        <v>2.97563155E-10</v>
+        <v>3.6461437209999998E-11</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5399,10 +5399,10 @@
         <v>47</v>
       </c>
       <c r="C219">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D219" s="2">
-        <v>4.0539180865000002E-10</v>
+        <v>2.97563155E-10</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
@@ -5413,10 +5413,10 @@
         <v>47</v>
       </c>
       <c r="C220">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D220" s="2">
-        <v>3.9706489465999998E-10</v>
+        <v>4.0539180865000002E-10</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5427,38 +5427,38 @@
         <v>47</v>
       </c>
       <c r="C221">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D221" s="2">
-        <v>4.5348227605999998E-10</v>
+        <v>3.9706489465999998E-10</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B222" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C222">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D222" s="2">
-        <v>3.8728284177000001E-10</v>
+        <v>4.5348227605999998E-10</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B223" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C223">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D223" s="2">
-        <v>1.4242893768E-12</v>
+        <v>3.8728284177000001E-10</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5469,10 +5469,10 @@
         <v>51</v>
       </c>
       <c r="C224">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D224" s="2">
-        <v>1.6973816083E-11</v>
+        <v>1.4242893768E-12</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5483,10 +5483,10 @@
         <v>51</v>
       </c>
       <c r="C225">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D225" s="2">
-        <v>3.5953079703999999E-10</v>
+        <v>1.6973816083E-11</v>
       </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
@@ -5497,10 +5497,10 @@
         <v>51</v>
       </c>
       <c r="C226">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D226" s="2">
-        <v>2.4689253438999998E-10</v>
+        <v>3.5953079703999999E-10</v>
       </c>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
@@ -5511,10 +5511,10 @@
         <v>51</v>
       </c>
       <c r="C227">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D227" s="2">
-        <v>2.9299711508999998E-10</v>
+        <v>2.4689253438999998E-10</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5525,38 +5525,38 @@
         <v>51</v>
       </c>
       <c r="C228">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D228" s="2">
-        <v>1.6385921765999999E-10</v>
+        <v>2.9299711508999998E-10</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B229" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C229">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D229" s="2">
-        <v>1.6536021062000001E-10</v>
+        <v>1.6385921765999999E-10</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B230" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C230">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D230" s="2">
-        <v>1.0840138722E-12</v>
+        <v>1.6536021062000001E-10</v>
       </c>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
@@ -5567,10 +5567,10 @@
         <v>55</v>
       </c>
       <c r="C231">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D231" s="2">
-        <v>2.7240150181000001E-11</v>
+        <v>1.0840138722E-12</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -5581,10 +5581,10 @@
         <v>55</v>
       </c>
       <c r="C232">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D232" s="2">
-        <v>1.2955417576999999E-10</v>
+        <v>2.7240150181000001E-11</v>
       </c>
     </row>
     <row r="233" spans="1:4" x14ac:dyDescent="0.25">
@@ -5595,10 +5595,10 @@
         <v>55</v>
       </c>
       <c r="C233">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D233" s="2">
-        <v>2.0060063853000001E-10</v>
+        <v>1.2955417576999999E-10</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
@@ -5609,10 +5609,10 @@
         <v>55</v>
       </c>
       <c r="C234">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D234" s="2">
-        <v>1.4976705546999999E-10</v>
+        <v>2.0060063853000001E-10</v>
       </c>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
@@ -5623,10 +5623,10 @@
         <v>55</v>
       </c>
       <c r="C235">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D235" s="2">
-        <v>2.9967498971999999E-10</v>
+        <v>1.4976705546999999E-10</v>
       </c>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
@@ -5637,24 +5637,24 @@
         <v>55</v>
       </c>
       <c r="C236">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D236" s="2">
-        <v>1.2302697120999999E-10</v>
+        <v>2.9967498971999999E-10</v>
       </c>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B237" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C237">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D237" s="2">
-        <v>1.6640141733000001E-10</v>
+        <v>1.2302697120999999E-10</v>
       </c>
     </row>
     <row r="238" spans="1:4" x14ac:dyDescent="0.25">
@@ -5665,24 +5665,24 @@
         <v>57</v>
       </c>
       <c r="C238">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D238" s="2">
-        <v>4.8571675403000001E-12</v>
+        <v>1.6640141733000001E-10</v>
       </c>
     </row>
     <row r="239" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A239">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C239">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D239" s="2">
-        <v>1.5509884903000001E-12</v>
+        <v>4.8571675403000001E-12</v>
       </c>
     </row>
     <row r="240" spans="1:4" x14ac:dyDescent="0.25">
@@ -5693,10 +5693,10 @@
         <v>59</v>
       </c>
       <c r="C240">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D240" s="2">
-        <v>5.0415159294E-11</v>
+        <v>1.5509884903000001E-12</v>
       </c>
     </row>
     <row r="241" spans="1:4" x14ac:dyDescent="0.25">
@@ -5707,10 +5707,10 @@
         <v>59</v>
       </c>
       <c r="C241">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D241" s="2">
-        <v>1.8120517446E-10</v>
+        <v>5.0415159294E-11</v>
       </c>
     </row>
     <row r="242" spans="1:4" x14ac:dyDescent="0.25">
@@ -5721,10 +5721,10 @@
         <v>59</v>
       </c>
       <c r="C242">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D242" s="2">
-        <v>2.6734941259000002E-10</v>
+        <v>1.8120517446E-10</v>
       </c>
     </row>
     <row r="243" spans="1:4" x14ac:dyDescent="0.25">
@@ -5735,10 +5735,10 @@
         <v>59</v>
       </c>
       <c r="C243">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D243" s="2">
-        <v>1.3423362999000001E-10</v>
+        <v>2.6734941259000002E-10</v>
       </c>
     </row>
     <row r="244" spans="1:4" x14ac:dyDescent="0.25">
@@ -5749,24 +5749,24 @@
         <v>59</v>
       </c>
       <c r="C244">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D244" s="2">
-        <v>3.4763535127999998E-10</v>
+        <v>1.3423362999000001E-10</v>
       </c>
     </row>
     <row r="245" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A245">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C245">
         <v>180</v>
       </c>
       <c r="D245" s="2">
-        <v>1.273497402E-14</v>
+        <v>3.4763535127999998E-10</v>
       </c>
     </row>
     <row r="246" spans="1:4" x14ac:dyDescent="0.25">
@@ -5777,24 +5777,24 @@
         <v>61</v>
       </c>
       <c r="C246">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D246" s="2">
-        <v>1.0670155991E-10</v>
+        <v>1.273497402E-14</v>
       </c>
     </row>
     <row r="247" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A247">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B247" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C247">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D247" s="2">
-        <v>1.1884969275E-12</v>
+        <v>1.0670155991E-10</v>
       </c>
     </row>
     <row r="248" spans="1:4" x14ac:dyDescent="0.25">
@@ -5805,10 +5805,10 @@
         <v>63</v>
       </c>
       <c r="C248">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D248" s="2">
-        <v>2.6537595745999998E-10</v>
+        <v>1.1884969275E-12</v>
       </c>
     </row>
     <row r="249" spans="1:4" x14ac:dyDescent="0.25">
@@ -5819,10 +5819,10 @@
         <v>63</v>
       </c>
       <c r="C249">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D249" s="2">
-        <v>1.4409039624E-10</v>
+        <v>2.6537595745999998E-10</v>
       </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
@@ -5833,10 +5833,10 @@
         <v>63</v>
       </c>
       <c r="C250">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D250" s="2">
-        <v>3.1020650174999998E-10</v>
+        <v>1.4409039624E-10</v>
       </c>
     </row>
     <row r="251" spans="1:4" x14ac:dyDescent="0.25">
@@ -5847,24 +5847,24 @@
         <v>63</v>
       </c>
       <c r="C251">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D251" s="2">
-        <v>2.9096055474000001E-10</v>
+        <v>3.1020650174999998E-10</v>
       </c>
     </row>
     <row r="252" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A252">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C252">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D252" s="2">
-        <v>9.3308613513999996E-11</v>
+        <v>2.9096055474000001E-10</v>
       </c>
     </row>
     <row r="253" spans="1:4" x14ac:dyDescent="0.25">
@@ -5875,24 +5875,24 @@
         <v>65</v>
       </c>
       <c r="C253">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D253" s="2">
-        <v>1.7015843205999999E-10</v>
+        <v>9.3308613513999996E-11</v>
       </c>
     </row>
     <row r="254" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A254">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C254">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D254" s="2">
-        <v>7.1844269091000003E-13</v>
+        <v>1.7015843205999999E-10</v>
       </c>
     </row>
     <row r="255" spans="1:4" x14ac:dyDescent="0.25">
@@ -5903,10 +5903,10 @@
         <v>67</v>
       </c>
       <c r="C255">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D255" s="2">
-        <v>5.8027522862000002E-11</v>
+        <v>7.1844269091000003E-13</v>
       </c>
     </row>
     <row r="256" spans="1:4" x14ac:dyDescent="0.25">
@@ -5917,10 +5917,10 @@
         <v>67</v>
       </c>
       <c r="C256">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D256" s="2">
-        <v>4.6401441154000002E-11</v>
+        <v>5.8027522862000002E-11</v>
       </c>
     </row>
     <row r="257" spans="1:4" x14ac:dyDescent="0.25">
@@ -5931,10 +5931,10 @@
         <v>67</v>
       </c>
       <c r="C257">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D257" s="2">
-        <v>4.895085847E-10</v>
+        <v>4.6401441154000002E-11</v>
       </c>
     </row>
     <row r="258" spans="1:4" x14ac:dyDescent="0.25">
@@ -5945,10 +5945,10 @@
         <v>67</v>
       </c>
       <c r="C258">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D258" s="2">
-        <v>6.0000292303999998E-10</v>
+        <v>4.895085847E-10</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -5959,10 +5959,10 @@
         <v>67</v>
       </c>
       <c r="C259">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D259" s="2">
-        <v>9.8090073872000002E-10</v>
+        <v>6.0000292303999998E-10</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -5973,24 +5973,24 @@
         <v>67</v>
       </c>
       <c r="C260">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D260" s="2">
-        <v>1.5019825369E-9</v>
+        <v>9.8090073872000002E-10</v>
       </c>
     </row>
     <row r="261" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A261">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B261" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C261">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D261" s="2">
-        <v>1.3282704505999999E-9</v>
+        <v>1.5019825369E-9</v>
       </c>
     </row>
     <row r="262" spans="1:4" x14ac:dyDescent="0.25">
@@ -6001,24 +6001,24 @@
         <v>69</v>
       </c>
       <c r="C262">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D262" s="2">
-        <v>2.2561561907999998E-9</v>
+        <v>1.3282704505999999E-9</v>
       </c>
     </row>
     <row r="263" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A263">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C263">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D263" s="2">
-        <v>8.6183861476000001E-13</v>
+        <v>2.2561561907999998E-9</v>
       </c>
     </row>
     <row r="264" spans="1:4" x14ac:dyDescent="0.25">
@@ -6029,10 +6029,10 @@
         <v>71</v>
       </c>
       <c r="C264">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D264" s="2">
-        <v>4.8646577810000003E-11</v>
+        <v>8.6183861476000001E-13</v>
       </c>
     </row>
     <row r="265" spans="1:4" x14ac:dyDescent="0.25">
@@ -6043,10 +6043,10 @@
         <v>71</v>
       </c>
       <c r="C265">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D265" s="2">
-        <v>2.0721704214E-9</v>
+        <v>4.8646577810000003E-11</v>
       </c>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
@@ -6057,10 +6057,10 @@
         <v>71</v>
       </c>
       <c r="C266">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D266" s="2">
-        <v>2.1375023244E-9</v>
+        <v>2.0721704214E-9</v>
       </c>
     </row>
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
@@ -6071,10 +6071,10 @@
         <v>71</v>
       </c>
       <c r="C267">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D267" s="2">
-        <v>1.6029653915000001E-9</v>
+        <v>2.1375023244E-9</v>
       </c>
     </row>
     <row r="268" spans="1:4" x14ac:dyDescent="0.25">
@@ -6085,38 +6085,38 @@
         <v>71</v>
       </c>
       <c r="C268">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D268" s="2">
-        <v>4.5952003741E-10</v>
+        <v>1.6029653915000001E-9</v>
       </c>
     </row>
     <row r="269" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A269">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B269" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C269">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D269" s="2">
-        <v>1.2735339834E-9</v>
+        <v>4.5952003741E-10</v>
       </c>
     </row>
     <row r="270" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A270">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B270" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C270">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D270" s="2">
-        <v>3.3798049880999998E-12</v>
+        <v>1.2735339834E-9</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -6127,10 +6127,10 @@
         <v>75</v>
       </c>
       <c r="C271">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D271" s="2">
-        <v>2.2693666104999999E-10</v>
+        <v>3.3798049880999998E-12</v>
       </c>
     </row>
     <row r="272" spans="1:4" x14ac:dyDescent="0.25">
@@ -6141,10 +6141,10 @@
         <v>75</v>
       </c>
       <c r="C272">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D272" s="2">
-        <v>3.8593349386999998E-10</v>
+        <v>2.2693666104999999E-10</v>
       </c>
     </row>
     <row r="273" spans="1:4" x14ac:dyDescent="0.25">
@@ -6155,10 +6155,10 @@
         <v>75</v>
       </c>
       <c r="C273">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D273" s="2">
-        <v>5.3111221240999998E-10</v>
+        <v>3.8593349386999998E-10</v>
       </c>
     </row>
     <row r="274" spans="1:4" x14ac:dyDescent="0.25">
@@ -6169,10 +6169,10 @@
         <v>75</v>
       </c>
       <c r="C274">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D274" s="2">
-        <v>3.0454801966999998E-10</v>
+        <v>5.3111221240999998E-10</v>
       </c>
     </row>
     <row r="275" spans="1:4" x14ac:dyDescent="0.25">
@@ -6183,10 +6183,10 @@
         <v>75</v>
       </c>
       <c r="C275">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D275" s="2">
-        <v>6.9340263069999998E-10</v>
+        <v>3.0454801966999998E-10</v>
       </c>
     </row>
     <row r="276" spans="1:4" x14ac:dyDescent="0.25">
@@ -6197,24 +6197,24 @@
         <v>75</v>
       </c>
       <c r="C276">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D276" s="2">
-        <v>1.6111323451000001E-10</v>
+        <v>6.9340263069999998E-10</v>
       </c>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A277">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B277" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C277">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="D277" s="2">
-        <v>3.7001177649000002E-10</v>
+        <v>1.6111323451000001E-10</v>
       </c>
     </row>
     <row r="278" spans="1:4" x14ac:dyDescent="0.25">
@@ -6225,24 +6225,24 @@
         <v>77</v>
       </c>
       <c r="C278">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D278" s="2">
-        <v>8.9194776192999999E-10</v>
+        <v>3.7001177649000002E-10</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A279">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B279" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C279">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D279" s="2">
-        <v>1.7805433202999999E-10</v>
+        <v>8.9194776192999999E-10</v>
       </c>
     </row>
     <row r="280" spans="1:4" x14ac:dyDescent="0.25">
@@ -6253,10 +6253,10 @@
         <v>79</v>
       </c>
       <c r="C280">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D280" s="2">
-        <v>1.6730310003000001E-9</v>
+        <v>1.7805433202999999E-10</v>
       </c>
     </row>
     <row r="281" spans="1:4" x14ac:dyDescent="0.25">
@@ -6267,10 +6267,10 @@
         <v>79</v>
       </c>
       <c r="C281">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D281" s="2">
-        <v>1.8603777345999999E-9</v>
+        <v>1.6730310003000001E-9</v>
       </c>
     </row>
     <row r="282" spans="1:4" x14ac:dyDescent="0.25">
@@ -6281,52 +6281,52 @@
         <v>79</v>
       </c>
       <c r="C282">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D282" s="2">
-        <v>5.3507313666000001E-9</v>
+        <v>1.8603777345999999E-9</v>
       </c>
     </row>
     <row r="283" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A283">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B283" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C283">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D283" s="2">
-        <v>7.2558884649000002E-10</v>
+        <v>5.3507313666000001E-9</v>
       </c>
     </row>
     <row r="284" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A284">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B284" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C284">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="D284" s="2">
-        <v>1.888131758E-10</v>
+        <v>7.2558884649000002E-10</v>
       </c>
     </row>
     <row r="285" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A285">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B285" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C285">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D285" s="2">
-        <v>1.0490354517E-15</v>
+        <v>1.888131758E-10</v>
       </c>
     </row>
     <row r="286" spans="1:4" x14ac:dyDescent="0.25">
@@ -6337,10 +6337,10 @@
         <v>85</v>
       </c>
       <c r="C286">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D286" s="2">
-        <v>1.2792875257000001E-11</v>
+        <v>1.0490354517E-15</v>
       </c>
     </row>
     <row r="287" spans="1:4" x14ac:dyDescent="0.25">
@@ -6351,9 +6351,23 @@
         <v>85</v>
       </c>
       <c r="C287">
+        <v>235</v>
+      </c>
+      <c r="D287" s="2">
+        <v>1.2792875257000001E-11</v>
+      </c>
+    </row>
+    <row r="288" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>92</v>
+      </c>
+      <c r="B288" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C288">
         <v>238</v>
       </c>
-      <c r="D287" s="2">
+      <c r="D288" s="2">
         <v>4.0391128556000002E-11</v>
       </c>
     </row>

</xml_diff>